<commit_message>
study population cohort addition
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_study_population_target_cohorts.xlsx
+++ b/i_codebooks/D3_study_population_target_cohorts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE243AAA-0E43-4502-9F8A-A8BEC4B87D19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="6900" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="6900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -18,19 +19,6 @@
     <sheet name="Example" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -260,12 +248,6 @@
     </r>
   </si>
   <si>
-    <t>for birth cohorts: the person is in the cohort if birth_date is between study_entry_date and study_exit_date
-for adolescence: the person is in the cohort if the ninth birthday is between study_entry_date and study_exit_date
-for seasonalXXX: the person is in the cohort if september (???) XXXX is between study_entry_date and study_exit_date
-forcovid_vacc: the person is in the cohort if 1st december 2020 is between study_entry_date and study_exit_date</t>
-  </si>
-  <si>
     <t>date of entry in the cohort cohort_type_and_label</t>
   </si>
   <si>
@@ -276,12 +258,6 @@
 for adolescence: ninth birthday 
 for seasonalXXX: september (???) XXXX 
 for covid_vacc: 1st december 2020</t>
-  </si>
-  <si>
-    <t>for birth cohorts: for birthYY, exit date is earliest between the date they turn XX months old and study_exit_date
-for adolescence: exit date is earliest between the date they turn 16 years old and study_exit_date
-for seasonalXXX: exit date is earliest between end of season (april?) and study_exit_date
-for covid_vacc: study_exit_date</t>
   </si>
   <si>
     <r>
@@ -469,11 +445,24 @@
   <si>
     <t>P003</t>
   </si>
+  <si>
+    <t>for birth cohorts: for birthYY, exit date is earliest between the date they turn XX months old and study_exit_date
+for adolescence: exit date is earliest between the date they turn 16 years old and study_exit_date
+for seasonalXXX: exit date is earliest between end of season 30th april XXXX and study_exit_date
+for covid_vacc: study_exit_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for birth cohorts: the person is in the cohort if birth_date is between study_entry_date and study_exit_date
+for adolescence: the person is in the cohort if the ninth birthday is between study_entry_date and study_exit_date
+for seasonalXXX: the person is in the cohort if 1st september XXXX is between study_entry_date and study_exit_date
+forcovid_vacc: the person is in the cohort if 1st december 2020 is between study_entry_date and study_exit_date
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -719,7 +708,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1030,20 +1019,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1059,7 +1048,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1075,12 +1064,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -1115,30 +1104,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A11"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="3"/>
-    <col min="4" max="4" width="34.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="83.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="23" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="34.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="83.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="44" style="3" customWidth="1"/>
-    <col min="7" max="10" width="9.109375" style="3"/>
-    <col min="11" max="11" width="35.77734375" style="14" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="3"/>
+    <col min="7" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="52.5703125" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1167,7 @@
       <c r="O1"/>
       <c r="P1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1235,7 +1224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -1264,12 +1253,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
@@ -1279,56 +1268,56 @@
       <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="144" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1338,22 +1327,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1356,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1381,7 +1370,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1384,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1409,7 +1398,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1423,7 +1412,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1437,7 +1426,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1451,7 +1440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1465,7 +1454,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1485,21 +1474,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AY4"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1519,141 +1508,141 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>73</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>76</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>78</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>79</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>80</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>81</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>86</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>87</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>88</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>90</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>91</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>92</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>93</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>94</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>95</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>96</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>100</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>101</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>103</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>105</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>106</v>
       </c>
-      <c r="AW1" t="s">
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>107</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>109</v>
       </c>
       <c r="B2">
         <v>20200101</v>
@@ -1725,9 +1714,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>20100101</v>
@@ -1781,9 +1770,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>19400101</v>
@@ -1906,15 +1895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -1924,6 +1904,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2172,14 +2161,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2192,6 +2173,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>